<commit_message>
eddy ni 1994-1995 (update 2)
</commit_message>
<xml_diff>
--- a/_data/ni/ni9495/individueel_eindstand_dworp_123_9495.xlsx
+++ b/_data/ni/ni9495/individueel_eindstand_dworp_123_9495.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="12840"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="12840" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="229">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -697,13 +697,25 @@
     <t>De Vleeschauwer Raoul</t>
   </si>
   <si>
-    <t>De Vriendt Augustin</t>
-  </si>
-  <si>
     <t>De Munck Jan</t>
   </si>
   <si>
     <t>De Saegher Johan</t>
+  </si>
+  <si>
+    <t>De Vriendt P</t>
+  </si>
+  <si>
+    <t>DEVRIENDT PATRICK</t>
+  </si>
+  <si>
+    <t>DEVRIENDT AUGUSTIN</t>
+  </si>
+  <si>
+    <t>elolijst januari 1995</t>
+  </si>
+  <si>
+    <t>Patrick is niet actief, elo blijft in latere lijsten ongewijzigd, dus het zou moeten Augustin zijn.</t>
   </si>
 </sst>
 </file>
@@ -801,7 +813,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -847,6 +859,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1305,7 +1323,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1492,6 +1510,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1795,7 +1815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3535,9 +3555,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3552,9 +3572,14 @@
     <col min="9" max="9" width="30.7109375" customWidth="1"/>
     <col min="10" max="10" width="6.7109375" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21">
+    <row r="1" spans="1:19" ht="21">
       <c r="A1" s="25" t="s">
         <v>30</v>
       </c>
@@ -3565,12 +3590,12 @@
         <v>34777</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="19.5" thickBot="1">
+    <row r="2" spans="1:19" ht="19.5" thickBot="1">
       <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:19">
       <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
         <v>11</v>
@@ -3590,7 +3615,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:19">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -3620,7 +3645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:19">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -3652,7 +3677,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:19">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -3684,7 +3709,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:19">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -3716,7 +3741,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:19">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -3748,7 +3773,7 @@
         <v>1895</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:19">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -3764,7 +3789,7 @@
       <c r="I9" s="14"/>
       <c r="J9" s="18"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1">
+    <row r="10" spans="1:19" ht="15.75" thickBot="1">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -3780,7 +3805,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="18"/>
     </row>
-    <row r="11" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+    <row r="11" spans="1:19" ht="16.5" thickTop="1" thickBot="1">
       <c r="A11" s="6"/>
       <c r="B11" s="3"/>
       <c r="C11" s="16">
@@ -3804,12 +3829,12 @@
       </c>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="19.5" thickBot="1">
+    <row r="12" spans="1:19" ht="19.5" thickBot="1">
       <c r="A12" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:19">
       <c r="A13" s="4"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
@@ -3829,7 +3854,7 @@
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:19">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -3859,7 +3884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:19">
       <c r="A15" s="5">
         <v>1</v>
       </c>
@@ -3890,20 +3915,20 @@
       <c r="J15" s="18">
         <v>1985</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="L15" s="70" t="s">
+        <v>227</v>
+      </c>
+      <c r="M15" s="70"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="5">
         <v>2</v>
       </c>
-      <c r="B16" s="19">
-        <v>62316</v>
-      </c>
+      <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="D16" s="18">
-        <v>1628</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="D16" s="18"/>
       <c r="E16" s="10">
         <v>0</v>
       </c>
@@ -3922,8 +3947,28 @@
       <c r="J16" s="18">
         <v>1862</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="L16" s="70">
+        <v>50288</v>
+      </c>
+      <c r="M16" s="70" t="s">
+        <v>225</v>
+      </c>
+      <c r="N16" s="70">
+        <v>408</v>
+      </c>
+      <c r="O16" s="71">
+        <v>20511</v>
+      </c>
+      <c r="P16" s="70">
+        <v>1726</v>
+      </c>
+      <c r="Q16" s="70">
+        <v>28</v>
+      </c>
+      <c r="R16" s="70"/>
+      <c r="S16" s="70"/>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="5">
         <v>3</v>
       </c>
@@ -3954,8 +3999,28 @@
       <c r="J17" s="18">
         <v>1768</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1">
+      <c r="L17" s="70">
+        <v>62316</v>
+      </c>
+      <c r="M17" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="N17" s="70">
+        <v>425</v>
+      </c>
+      <c r="O17" s="71">
+        <v>21199</v>
+      </c>
+      <c r="P17" s="70">
+        <v>1628</v>
+      </c>
+      <c r="Q17" s="70">
+        <v>391</v>
+      </c>
+      <c r="R17" s="70"/>
+      <c r="S17" s="70"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" thickBot="1">
       <c r="A18" s="5">
         <v>4</v>
       </c>
@@ -3986,13 +4051,23 @@
       <c r="J18" s="18">
         <v>1708</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="L18" s="70" t="s">
+        <v>228</v>
+      </c>
+      <c r="M18" s="70"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="70"/>
+      <c r="P18" s="70"/>
+      <c r="Q18" s="70"/>
+      <c r="R18" s="70"/>
+      <c r="S18" s="70"/>
+    </row>
+    <row r="19" spans="1:19" ht="16.5" thickTop="1" thickBot="1">
       <c r="A19" s="6"/>
       <c r="B19" s="3"/>
       <c r="C19" s="16">
         <f>IFERROR(AVERAGE(D15:D18),"")</f>
-        <v>1675.25</v>
+        <v>1691</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="13">
@@ -4011,12 +4086,12 @@
       </c>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="19.5" thickBot="1">
+    <row r="20" spans="1:19" ht="19.5" thickBot="1">
       <c r="A20" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:19">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>11</v>
@@ -4036,7 +4111,7 @@
       </c>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:19">
       <c r="A22" s="5" t="s">
         <v>5</v>
       </c>
@@ -4066,7 +4141,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:19">
       <c r="A23" s="5">
         <v>1</v>
       </c>
@@ -4098,7 +4173,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:19">
       <c r="A24" s="5">
         <v>2</v>
       </c>
@@ -4130,7 +4205,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:19">
       <c r="A25" s="5">
         <v>3</v>
       </c>
@@ -4162,7 +4237,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1">
+    <row r="26" spans="1:19" ht="15.75" thickBot="1">
       <c r="A26" s="5">
         <v>4</v>
       </c>
@@ -4194,7 +4269,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+    <row r="27" spans="1:19" ht="16.5" thickTop="1" thickBot="1">
       <c r="A27" s="6"/>
       <c r="B27" s="3"/>
       <c r="C27" s="16">
@@ -4218,12 +4293,12 @@
       </c>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" ht="19.5" thickBot="1">
+    <row r="28" spans="1:19" ht="19.5" thickBot="1">
       <c r="A28" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:19">
       <c r="A29" s="4"/>
       <c r="B29" s="2" t="s">
         <v>11</v>
@@ -4239,7 +4314,7 @@
       <c r="I29" s="15"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:19">
       <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
@@ -4269,7 +4344,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:19">
       <c r="A31" s="5">
         <v>1</v>
       </c>
@@ -4285,7 +4360,7 @@
       <c r="I31" s="14"/>
       <c r="J31" s="18"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:19">
       <c r="A32" s="5">
         <v>2</v>
       </c>
@@ -15952,7 +16027,7 @@
         <v>21938</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D15" s="18">
         <v>2063</v>
@@ -15984,7 +16059,7 @@
         <v>21717</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D16" s="18">
         <v>2028</v>

</xml_diff>